<commit_message>
set of counteragents added
</commit_message>
<xml_diff>
--- a/app/files/expenses.xlsx
+++ b/app/files/expenses.xlsx
@@ -544,7 +544,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>3651</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="7">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>6524</v>
+        <v>7831</v>
       </c>
     </row>
     <row r="9">
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>1047</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="12">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>1090</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="13">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>1090</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="14">
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>1090</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="15">
@@ -706,7 +706,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>733</v>
+        <v>880</v>
       </c>
     </row>
     <row r="16">
@@ -724,7 +724,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>707</v>
+        <v>849</v>
       </c>
     </row>
     <row r="17">
@@ -742,7 +742,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>707</v>
+        <v>849</v>
       </c>
     </row>
     <row r="18">
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>707</v>
+        <v>849</v>
       </c>
     </row>
     <row r="19">
@@ -778,7 +778,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>707</v>
+        <v>849</v>
       </c>
     </row>
     <row r="20">
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>707</v>
+        <v>849</v>
       </c>
     </row>
     <row r="21">
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>707</v>
+        <v>849</v>
       </c>
     </row>
     <row r="22">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>707</v>
+        <v>849</v>
       </c>
     </row>
     <row r="23">
@@ -868,7 +868,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>2301</v>
+        <v>2761</v>
       </c>
     </row>
     <row r="25">
@@ -886,7 +886,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>2419</v>
+        <v>2903</v>
       </c>
     </row>
     <row r="26">
@@ -904,7 +904,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>2170</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="27">
@@ -922,7 +922,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>2103</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="28">
@@ -940,7 +940,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>2103</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="29">
@@ -958,7 +958,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>2103</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="30">
@@ -976,7 +976,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>2103</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="31">
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>2103</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="32">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>2103</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="33">
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>2103</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="34">
@@ -1048,7 +1048,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>2103</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="35">
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>2103</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="36">
@@ -1156,7 +1156,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>46664</v>
+        <v>56000</v>
       </c>
     </row>
     <row r="41">
@@ -1174,7 +1174,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>497954</v>
+        <v>597545</v>
       </c>
     </row>
     <row r="42">
@@ -1264,7 +1264,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>155494</v>
+        <v>186600</v>
       </c>
     </row>
     <row r="47">
@@ -1282,7 +1282,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>50458</v>
+        <v>60550</v>
       </c>
     </row>
     <row r="48">
@@ -1714,7 +1714,7 @@
         </is>
       </c>
       <c r="E71" t="n">
-        <v>169968</v>
+        <v>203962</v>
       </c>
     </row>
     <row r="72">
@@ -1858,7 +1858,7 @@
         </is>
       </c>
       <c r="E79" t="n">
-        <v>9583</v>
+        <v>11500</v>
       </c>
     </row>
     <row r="80">
@@ -1876,7 +1876,7 @@
         </is>
       </c>
       <c r="E80" t="n">
-        <v>5775</v>
+        <v>6930</v>
       </c>
     </row>
     <row r="81">
@@ -2218,7 +2218,7 @@
         </is>
       </c>
       <c r="E99" t="n">
-        <v>9916</v>
+        <v>11900</v>
       </c>
     </row>
     <row r="100">
@@ -2236,7 +2236,7 @@
         </is>
       </c>
       <c r="E100" t="n">
-        <v>23332</v>
+        <v>26833</v>
       </c>
     </row>
     <row r="101">
@@ -2254,7 +2254,7 @@
         </is>
       </c>
       <c r="E101" t="n">
-        <v>252051</v>
+        <v>302461</v>
       </c>
     </row>
     <row r="102">
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="E103" t="n">
-        <v>12916</v>
+        <v>15500</v>
       </c>
     </row>
     <row r="104">
@@ -2308,7 +2308,7 @@
         </is>
       </c>
       <c r="E104" t="n">
-        <v>22131</v>
+        <v>26557</v>
       </c>
     </row>
     <row r="105">
@@ -2380,7 +2380,7 @@
         </is>
       </c>
       <c r="E108" t="n">
-        <v>18059</v>
+        <v>21671</v>
       </c>
     </row>
     <row r="109">
@@ -2452,7 +2452,7 @@
         </is>
       </c>
       <c r="E112" t="n">
-        <v>37500</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="113">
@@ -2488,7 +2488,7 @@
         </is>
       </c>
       <c r="E114" t="n">
-        <v>3733</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="115">
@@ -2524,7 +2524,7 @@
         </is>
       </c>
       <c r="E116" t="n">
-        <v>10500</v>
+        <v>12600</v>
       </c>
     </row>
     <row r="117">
@@ -2560,7 +2560,7 @@
         </is>
       </c>
       <c r="E118" t="n">
-        <v>112500</v>
+        <v>135000</v>
       </c>
     </row>
     <row r="119">
@@ -2578,7 +2578,7 @@
         </is>
       </c>
       <c r="E119" t="n">
-        <v>7083</v>
+        <v>8500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>